<commit_message>
Updated shape files for Oak Creek
</commit_message>
<xml_diff>
--- a/Retreat_Fire_2024/site_selection/Scouting/Oak_Creek_tribs_scouting.xlsx
+++ b/Retreat_Fire_2024/site_selection/Scouting/Oak_Creek_tribs_scouting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-fire-watch/Retreat_Fire_2024/site_selection/Scouting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AD0E07C-752C-154F-8BC6-76F40CA8B32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13D594B-10D8-764D-82CF-1C5FBCD0EC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="760" windowWidth="27640" windowHeight="16700" xr2:uid="{E8F89692-5212-0240-9481-0B9728A709FA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{E8F89692-5212-0240-9481-0B9728A709FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Oak_Creek_tribs_scouting" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>site</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t>Moderate_Low</t>
+  </si>
+  <si>
+    <t></t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +118,23 @@
     </font>
     <font>
       <u/>
+      <sz val="12"/>
+      <color rgb="FF1A73E8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Google Symbols"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF1A73E8"/>
       <name val="Arial"/>
@@ -141,9 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,13 +501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D8F72B-54BC-9646-8A99-4032849CCFAB}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="6" max="6" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -492,7 +515,7 @@
     <col min="9" max="10" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,15 +550,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>46.729877999999999</v>
+        <v>46.729033999999999</v>
       </c>
       <c r="C2">
-        <v>-120.851257</v>
+        <v>-120.850735</v>
       </c>
       <c r="E2">
         <v>24424741</v>
@@ -556,15 +579,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>46.731318000000002</v>
+        <v>46.730728999999997</v>
       </c>
       <c r="C3">
-        <v>-120.861048</v>
+        <v>-120.861149</v>
       </c>
       <c r="E3">
         <v>24424729</v>
@@ -585,15 +608,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>46.73254</v>
+        <v>46.731386000000001</v>
       </c>
       <c r="C4">
-        <v>-120.87936000000001</v>
+        <v>-120.87894</v>
       </c>
       <c r="E4">
         <v>24424727</v>
@@ -613,16 +636,17 @@
       <c r="J4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="18">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>46.737779000000003</v>
+        <v>46.735142000000003</v>
       </c>
       <c r="C5">
-        <v>-120.907821</v>
+        <v>-120.907946</v>
       </c>
       <c r="E5">
         <v>24424705</v>
@@ -642,16 +666,17 @@
       <c r="J5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="23">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>46.738840000000003</v>
+        <v>46.73563</v>
       </c>
       <c r="C6">
-        <v>-120.926922</v>
+        <v>-120.923647</v>
       </c>
       <c r="E6">
         <v>24424703</v>
@@ -671,16 +696,19 @@
       <c r="J6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>46.729807000000001</v>
+        <v>46.730606999999999</v>
       </c>
       <c r="C7">
-        <v>-120.950459</v>
+        <v>-120.949185</v>
       </c>
       <c r="E7">
         <v>24424717</v>
@@ -701,15 +729,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="23">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>46.725326000000003</v>
+        <v>46.725380000000001</v>
       </c>
       <c r="C8">
-        <v>-120.94154</v>
+        <v>-120.941457</v>
       </c>
       <c r="E8">
         <v>24424753</v>
@@ -729,8 +757,19 @@
       <c r="J8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18">
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="23">
+      <c r="N10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="F16" s="1"/>
     </row>
   </sheetData>

</xml_diff>